<commit_message>
make Excelable trait for fetching prices from excel files
</commit_message>
<xml_diff>
--- a/public/excel/0.5.xlsx
+++ b/public/excel/0.5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="648"/>
   </bookViews>
   <sheets>
     <sheet name="Трубы голые" sheetId="19" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="143">
   <si>
     <t>Волпер</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>Колено 45 нерж\оц</t>
+  </si>
+  <si>
+    <t>elements</t>
   </si>
 </sst>
 </file>
@@ -8150,8 +8153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="170" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8161,7 +8164,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>13</v>
+        <v>142</v>
       </c>
       <c r="B1" s="29">
         <v>100</v>
@@ -9407,8 +9410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="159" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="159" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9418,7 +9421,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>13</v>
+        <v>142</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
fix a couple of styles and add meta tags for yandex search engine
</commit_message>
<xml_diff>
--- a/public/excel/0.5.xlsx
+++ b/public/excel/0.5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="141">
   <si>
     <t>Волпер</t>
   </si>
@@ -129,12 +129,6 @@
   </si>
   <si>
     <t>500/560</t>
-  </si>
-  <si>
-    <t>Труба 0,5м нерж\нерж</t>
-  </si>
-  <si>
-    <t>Труба 0,25м нерж\нерж</t>
   </si>
   <si>
     <t>Ревизия нерж\нерж</t>
@@ -401,37 +395,10 @@
     <t>Труба 1м</t>
   </si>
   <si>
-    <t>Труба 0,5м</t>
-  </si>
-  <si>
-    <t>Труба 0,3м</t>
-  </si>
-  <si>
-    <t>Колено 90</t>
-  </si>
-  <si>
-    <t>Колено 45</t>
-  </si>
-  <si>
-    <t>Тройник 87</t>
-  </si>
-  <si>
-    <t>Тройник 45</t>
-  </si>
-  <si>
     <t>Скоба крепёжная</t>
   </si>
   <si>
-    <t>Труба 0,25м нерж\оц</t>
-  </si>
-  <si>
-    <t>Труба 0,5м нерж\оц</t>
-  </si>
-  <si>
     <t>Труба 1м нерж\оц</t>
-  </si>
-  <si>
-    <t>Труба 1м нерж\нерж</t>
   </si>
   <si>
     <t>Ревизия нерж\оц</t>
@@ -440,31 +407,58 @@
     <t>Конус термо нерж\оц</t>
   </si>
   <si>
-    <t>Тройник 87 нерж\нерж</t>
+    <t>elements</t>
   </si>
   <si>
-    <t>Тройник 87 нерж\оц</t>
+    <t>Труба 1м нерж\нерж</t>
   </si>
   <si>
-    <t>Тройник 45 нерж\нерж</t>
+    <t>Тройник 87* нерж\нерж</t>
   </si>
   <si>
-    <t>Тройник 45 нерж\оц</t>
+    <t>Тройник 87* нерж\оц</t>
   </si>
   <si>
-    <t>Колено 90 нерж\нерж</t>
+    <t>Тройник 45* нерж\нерж</t>
   </si>
   <si>
-    <t>Колено 90 нерж\оц</t>
+    <t>Тройник 45* нерж\оц</t>
   </si>
   <si>
-    <t>Колено 45 нерж\нерж</t>
+    <t>Колено 90* нерж\нерж</t>
   </si>
   <si>
-    <t>Колено 45 нерж\оц</t>
+    <t>Колено 90* нерж\оц</t>
   </si>
   <si>
-    <t>elements</t>
+    <t>Колено 45* нерж\нерж</t>
+  </si>
+  <si>
+    <t>Колено 45* нерж\оц</t>
+  </si>
+  <si>
+    <t>Тройник 87*</t>
+  </si>
+  <si>
+    <t>Тройник 45*</t>
+  </si>
+  <si>
+    <t>Труба 0.5м нерж\нерж</t>
+  </si>
+  <si>
+    <t>Труба 0.5м нерж\оц</t>
+  </si>
+  <si>
+    <t>Труба 0.25м нерж\нерж</t>
+  </si>
+  <si>
+    <t>Труба 0.25м нерж\оц</t>
+  </si>
+  <si>
+    <t>Труба 0.5м</t>
+  </si>
+  <si>
+    <t>Труба 0.3м</t>
   </si>
 </sst>
 </file>
@@ -8153,8 +8147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8164,7 +8158,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B1" s="29">
         <v>100</v>
@@ -8223,7 +8217,7 @@
     </row>
     <row r="2" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" s="46">
         <v>194.12</v>
@@ -8282,7 +8276,7 @@
     </row>
     <row r="3" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="B3" s="46">
         <v>96.600000000000009</v>
@@ -8341,7 +8335,7 @@
     </row>
     <row r="4" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="B4" s="46">
         <v>72</v>
@@ -8400,7 +8394,7 @@
     </row>
     <row r="5" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="B5" s="46">
         <v>177</v>
@@ -8459,7 +8453,7 @@
     </row>
     <row r="6" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
       <c r="B6" s="46">
         <v>83</v>
@@ -8518,7 +8512,7 @@
     </row>
     <row r="7" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B7" s="46">
         <v>211</v>
@@ -8577,7 +8571,7 @@
     </row>
     <row r="8" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B8" s="46">
         <v>248</v>
@@ -9038,13 +9032,13 @@
         <v>1525</v>
       </c>
       <c r="Q15" s="46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R15" s="46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S15" s="46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.2">
@@ -9226,7 +9220,7 @@
     </row>
     <row r="19" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B19" s="46">
         <v>47</v>
@@ -9410,8 +9404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView zoomScale="159" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="134" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9421,72 +9415,72 @@
   <sheetData>
     <row r="1" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="L1" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="O1" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="P1" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="Q1" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="R1" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="S1" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="T1" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="U1" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="U1" s="17" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B2" s="47">
         <v>514.28</v>
@@ -9551,7 +9545,7 @@
     </row>
     <row r="3" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B3" s="47">
         <v>372.6</v>
@@ -9616,7 +9610,7 @@
     </row>
     <row r="4" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="B4" s="47">
         <v>338.56</v>
@@ -9681,7 +9675,7 @@
     </row>
     <row r="5" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B5" s="47">
         <v>240.12</v>
@@ -9746,7 +9740,7 @@
     </row>
     <row r="6" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
       <c r="B6" s="47">
         <v>225</v>
@@ -9811,7 +9805,7 @@
     </row>
     <row r="7" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B7" s="47">
         <v>176</v>
@@ -9876,7 +9870,7 @@
     </row>
     <row r="8" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B8" s="47">
         <v>663.58089763779526</v>
@@ -9941,7 +9935,7 @@
     </row>
     <row r="9" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B9" s="47">
         <v>534.58089763779526</v>
@@ -10006,7 +10000,7 @@
     </row>
     <row r="10" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B10" s="47">
         <v>819.9656535433071</v>
@@ -10071,7 +10065,7 @@
     </row>
     <row r="11" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B11" s="47">
         <v>659.9656535433071</v>
@@ -10136,7 +10130,7 @@
     </row>
     <row r="12" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B12" s="47">
         <v>625</v>
@@ -10201,7 +10195,7 @@
     </row>
     <row r="13" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B13" s="47">
         <v>510</v>
@@ -10266,7 +10260,7 @@
     </row>
     <row r="14" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B14" s="47">
         <v>353.2</v>
@@ -10331,7 +10325,7 @@
     </row>
     <row r="15" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B15" s="47">
         <v>290.2</v>
@@ -10396,7 +10390,7 @@
     </row>
     <row r="16" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="47">
         <v>628</v>
@@ -10461,7 +10455,7 @@
     </row>
     <row r="17" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B17" s="47">
         <v>499</v>
@@ -10526,7 +10520,7 @@
     </row>
     <row r="18" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="47">
         <v>232</v>
@@ -10591,7 +10585,7 @@
     </row>
     <row r="19" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" s="47">
         <v>274</v>
@@ -10656,7 +10650,7 @@
     </row>
     <row r="20" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B20" s="47">
         <v>255</v>
@@ -10721,7 +10715,7 @@
     </row>
     <row r="21" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="47">
         <v>209</v>
@@ -10760,19 +10754,19 @@
         <v>535</v>
       </c>
       <c r="N21" s="47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O21" s="47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P21" s="47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q21" s="47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R21" s="47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S21" s="47">
         <v>256</v>
@@ -10786,7 +10780,7 @@
     </row>
     <row r="22" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" s="47">
         <v>763</v>
@@ -10831,13 +10825,13 @@
         <v>2994</v>
       </c>
       <c r="P22" s="47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q22" s="47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R22" s="47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S22" s="47">
         <v>836</v>
@@ -10851,7 +10845,7 @@
     </row>
     <row r="23" spans="1:21" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="47">
         <v>432</v>
@@ -10940,7 +10934,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -11011,7 +11005,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="62" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="63"/>
       <c r="D4" s="63"/>
@@ -11111,7 +11105,7 @@
     </row>
     <row r="7" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="38">
         <v>49</v>
@@ -11170,7 +11164,7 @@
     </row>
     <row r="8" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="38">
         <v>32</v>
@@ -11229,7 +11223,7 @@
     </row>
     <row r="9" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="38">
         <v>22</v>
@@ -11288,7 +11282,7 @@
     </row>
     <row r="10" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="38">
         <v>261</v>
@@ -11347,7 +11341,7 @@
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="38">
         <v>171</v>
@@ -11406,7 +11400,7 @@
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" s="38">
         <v>139</v>
@@ -11465,7 +11459,7 @@
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="38">
         <v>46</v>
@@ -11524,7 +11518,7 @@
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="38">
         <v>195</v>
@@ -11583,7 +11577,7 @@
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" s="38">
         <v>34</v>
@@ -11642,7 +11636,7 @@
     </row>
     <row r="16" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="38">
         <v>132</v>
@@ -11701,7 +11695,7 @@
     </row>
     <row r="17" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" s="38">
         <v>66</v>
@@ -11760,7 +11754,7 @@
     </row>
     <row r="18" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18" s="38">
         <v>80</v>
@@ -11819,7 +11813,7 @@
     </row>
     <row r="19" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" s="38">
         <v>337</v>
@@ -11878,7 +11872,7 @@
     </row>
     <row r="20" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20" s="38">
         <v>32</v>
@@ -11937,7 +11931,7 @@
     </row>
     <row r="21" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" s="38">
         <v>32</v>
@@ -11996,7 +11990,7 @@
     </row>
     <row r="22" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="38">
         <v>107</v>
@@ -12114,7 +12108,7 @@
     </row>
     <row r="24" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="42">
         <v>61</v>
@@ -12236,7 +12230,7 @@
     </row>
     <row r="28" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="54" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B28" s="55"/>
       <c r="C28" s="55"/>
@@ -12337,7 +12331,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" s="70" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" s="71"/>
       <c r="C2" s="71"/>
@@ -12382,7 +12376,7 @@
     </row>
     <row r="4" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="73" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="74"/>
       <c r="C4" s="74"/>
@@ -12428,7 +12422,7 @@
     </row>
     <row r="6" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>14</v>
@@ -12440,7 +12434,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>17</v>
@@ -12487,7 +12481,7 @@
     </row>
     <row r="7" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="19">
         <v>567</v>
@@ -12546,7 +12540,7 @@
     </row>
     <row r="8" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="19">
         <v>334</v>
@@ -12605,7 +12599,7 @@
     </row>
     <row r="9" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" s="19">
         <v>164</v>
@@ -12664,7 +12658,7 @@
     </row>
     <row r="10" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" s="19">
         <v>668</v>
@@ -12723,7 +12717,7 @@
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="19">
         <v>802</v>
@@ -12782,7 +12776,7 @@
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="19">
         <v>545</v>
@@ -12841,7 +12835,7 @@
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="19">
         <v>304</v>
@@ -12900,7 +12894,7 @@
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="19">
         <v>567</v>
@@ -12959,7 +12953,7 @@
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="19">
         <v>273</v>
@@ -13018,7 +13012,7 @@
     </row>
     <row r="16" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B16" s="19">
         <v>279</v>
@@ -13077,7 +13071,7 @@
     </row>
     <row r="17" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" s="19">
         <v>71</v>
@@ -13178,7 +13172,7 @@
     </row>
     <row r="20" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B20" s="57"/>
       <c r="C20" s="57"/>
@@ -13236,7 +13230,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" s="80" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -13259,7 +13253,7 @@
     </row>
     <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
@@ -13318,7 +13312,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>17</v>
@@ -13365,7 +13359,7 @@
     </row>
     <row r="5" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="24">
         <v>832</v>
@@ -13424,7 +13418,7 @@
     </row>
     <row r="6" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="24">
         <v>467</v>
@@ -13483,7 +13477,7 @@
     </row>
     <row r="7" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="24">
         <v>342</v>
@@ -13542,7 +13536,7 @@
     </row>
     <row r="8" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="24">
         <v>1644</v>
@@ -13601,7 +13595,7 @@
     </row>
     <row r="9" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="24">
         <v>939</v>
@@ -13660,7 +13654,7 @@
     </row>
     <row r="10" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10" s="24">
         <v>606</v>
@@ -13719,7 +13713,7 @@
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11" s="24">
         <v>541</v>
@@ -13778,7 +13772,7 @@
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" s="24">
         <v>1489</v>
@@ -13837,7 +13831,7 @@
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" s="24">
         <v>282</v>
@@ -13896,7 +13890,7 @@
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B14" s="24">
         <v>877</v>
@@ -13955,7 +13949,7 @@
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B15" s="24">
         <v>832</v>
@@ -14014,7 +14008,7 @@
     </row>
     <row r="16" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B16" s="24">
         <v>972</v>
@@ -14073,7 +14067,7 @@
     </row>
     <row r="17" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B17" s="24">
         <v>2014</v>
@@ -14132,7 +14126,7 @@
     </row>
     <row r="18" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" s="24">
         <v>2014</v>
@@ -14191,7 +14185,7 @@
     </row>
     <row r="19" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" s="24">
         <v>2063</v>
@@ -14250,7 +14244,7 @@
     </row>
     <row r="20" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B20" s="24">
         <v>203</v>
@@ -14309,7 +14303,7 @@
     </row>
     <row r="21" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" s="24">
         <v>398</v>
@@ -14368,7 +14362,7 @@
     </row>
     <row r="22" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" s="24">
         <v>479</v>
@@ -14427,7 +14421,7 @@
     </row>
     <row r="23" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B23" s="24">
         <v>809</v>
@@ -14486,7 +14480,7 @@
     </row>
     <row r="24" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B24" s="24">
         <v>681</v>
@@ -14545,7 +14539,7 @@
     </row>
     <row r="25" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B25" s="24">
         <v>387</v>
@@ -14604,7 +14598,7 @@
     </row>
     <row r="26" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B26" s="24">
         <v>1145</v>
@@ -14649,21 +14643,21 @@
         <v>3843</v>
       </c>
       <c r="P26" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q26" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R26" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S26" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B27" s="24">
         <v>1404</v>
@@ -14708,75 +14702,75 @@
         <v>4721</v>
       </c>
       <c r="P27" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q27" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R27" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S27" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="N28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S28" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="18" x14ac:dyDescent="0.2">
@@ -14802,7 +14796,7 @@
     </row>
     <row r="30" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="77" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B30" s="78"/>
       <c r="C30" s="78"/>

</xml_diff>

<commit_message>
make prices table expand
</commit_message>
<xml_diff>
--- a/public/excel/0.5.xlsx
+++ b/public/excel/0.5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="648"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Трубы голые" sheetId="19" r:id="rId1"/>
@@ -917,7 +917,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1035,9 +1035,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8147,8 +8144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9404,8 +9401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView zoomScale="134" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9482,64 +9479,64 @@
       <c r="A2" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="19">
         <v>514.28</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="19">
         <v>594.32000000000005</v>
       </c>
-      <c r="D2" s="47">
+      <c r="D2" s="19">
         <v>612.72</v>
       </c>
-      <c r="E2" s="47">
+      <c r="E2" s="19">
         <v>657.80000000000007</v>
       </c>
-      <c r="F2" s="47">
+      <c r="F2" s="19">
         <v>684.48</v>
       </c>
-      <c r="G2" s="47">
+      <c r="G2" s="19">
         <v>727.72</v>
       </c>
-      <c r="H2" s="47">
+      <c r="H2" s="19">
         <v>781.08</v>
       </c>
-      <c r="I2" s="47">
+      <c r="I2" s="19">
         <v>845.48</v>
       </c>
-      <c r="J2" s="47">
+      <c r="J2" s="19">
         <v>908.96</v>
       </c>
-      <c r="K2" s="47">
+      <c r="K2" s="19">
         <v>1005.5600000000001</v>
       </c>
-      <c r="L2" s="47">
+      <c r="L2" s="19">
         <v>1056.1600000000001</v>
       </c>
-      <c r="M2" s="47">
+      <c r="M2" s="19">
         <v>1334.92</v>
       </c>
-      <c r="N2" s="47">
+      <c r="N2" s="19">
         <v>1695.5600000000002</v>
       </c>
-      <c r="O2" s="47">
+      <c r="O2" s="19">
         <v>1962.3600000000001</v>
       </c>
-      <c r="P2" s="47">
+      <c r="P2" s="19">
         <v>2224.56</v>
       </c>
-      <c r="Q2" s="47">
+      <c r="Q2" s="19">
         <v>2519.88</v>
       </c>
-      <c r="R2" s="47">
+      <c r="R2" s="19">
         <v>2780.2400000000002</v>
       </c>
-      <c r="S2" s="47">
+      <c r="S2" s="19">
         <v>617.32000000000005</v>
       </c>
-      <c r="T2" s="47">
+      <c r="T2" s="19">
         <v>775.56000000000006</v>
       </c>
-      <c r="U2" s="47">
+      <c r="U2" s="19">
         <v>839.96</v>
       </c>
     </row>
@@ -9547,64 +9544,64 @@
       <c r="A3" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="19">
         <v>372.6</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="19">
         <v>408.48</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="19">
         <v>420.44</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="19">
         <v>459.08000000000004</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="19">
         <v>486.68</v>
       </c>
-      <c r="G3" s="47">
+      <c r="G3" s="19">
         <v>510.6</v>
       </c>
-      <c r="H3" s="47">
+      <c r="H3" s="19">
         <v>540.96</v>
       </c>
-      <c r="I3" s="47">
+      <c r="I3" s="19">
         <v>589.72</v>
       </c>
-      <c r="J3" s="47">
+      <c r="J3" s="19">
         <v>631.12</v>
       </c>
-      <c r="K3" s="47">
+      <c r="K3" s="19">
         <v>763.6</v>
       </c>
-      <c r="L3" s="47">
+      <c r="L3" s="19">
         <v>806.84</v>
       </c>
-      <c r="M3" s="47">
+      <c r="M3" s="19">
         <v>994.5200000000001</v>
       </c>
-      <c r="N3" s="47">
+      <c r="N3" s="19">
         <v>1357.92</v>
       </c>
-      <c r="O3" s="47">
+      <c r="O3" s="19">
         <v>1547.44</v>
       </c>
-      <c r="P3" s="47">
+      <c r="P3" s="19">
         <v>1759.96</v>
       </c>
-      <c r="Q3" s="47">
+      <c r="Q3" s="19">
         <v>1955.92</v>
       </c>
-      <c r="R3" s="47">
+      <c r="R3" s="19">
         <v>2119.6800000000003</v>
       </c>
-      <c r="S3" s="47">
+      <c r="S3" s="19">
         <v>458.16</v>
       </c>
-      <c r="T3" s="47">
+      <c r="T3" s="19">
         <v>506.92</v>
       </c>
-      <c r="U3" s="47">
+      <c r="U3" s="19">
         <v>547.4</v>
       </c>
     </row>
@@ -9612,64 +9609,64 @@
       <c r="A4" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="19">
         <v>338.56</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="19">
         <v>391</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="19">
         <v>402.04</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="19">
         <v>432.40000000000003</v>
       </c>
-      <c r="F4" s="47">
+      <c r="F4" s="19">
         <v>447.12</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="19">
         <v>469.20000000000005</v>
       </c>
-      <c r="H4" s="47">
+      <c r="H4" s="19">
         <v>514.28</v>
       </c>
-      <c r="I4" s="47">
+      <c r="I4" s="19">
         <v>545.56000000000006</v>
       </c>
-      <c r="J4" s="47">
+      <c r="J4" s="19">
         <v>587.88</v>
       </c>
-      <c r="K4" s="47">
+      <c r="K4" s="19">
         <v>652.28</v>
       </c>
-      <c r="L4" s="47">
+      <c r="L4" s="19">
         <v>684.48</v>
       </c>
-      <c r="M4" s="47">
+      <c r="M4" s="19">
         <v>872.16000000000008</v>
       </c>
-      <c r="N4" s="47">
+      <c r="N4" s="19">
         <v>1108.6000000000001</v>
       </c>
-      <c r="O4" s="47">
+      <c r="O4" s="19">
         <v>1274.2</v>
       </c>
-      <c r="P4" s="47">
+      <c r="P4" s="19">
         <v>1447.16</v>
       </c>
-      <c r="Q4" s="47">
+      <c r="Q4" s="19">
         <v>1637.6000000000001</v>
       </c>
-      <c r="R4" s="47">
+      <c r="R4" s="19">
         <v>1810.5600000000002</v>
       </c>
-      <c r="S4" s="47">
+      <c r="S4" s="19">
         <v>393.76</v>
       </c>
-      <c r="T4" s="47">
+      <c r="T4" s="19">
         <v>487.6</v>
       </c>
-      <c r="U4" s="47">
+      <c r="U4" s="19">
         <v>517.04000000000008</v>
       </c>
     </row>
@@ -9677,64 +9674,64 @@
       <c r="A5" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="19">
         <v>240.12</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="19">
         <v>266.8</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="19">
         <v>276.92</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="19">
         <v>300.84000000000003</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F5" s="19">
         <v>314.64</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G5" s="19">
         <v>338.56</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H5" s="19">
         <v>346.84000000000003</v>
       </c>
-      <c r="I5" s="47">
+      <c r="I5" s="19">
         <v>384.56</v>
       </c>
-      <c r="J5" s="47">
+      <c r="J5" s="19">
         <v>412.16</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K5" s="19">
         <v>503.24</v>
       </c>
-      <c r="L5" s="47">
+      <c r="L5" s="19">
         <v>527.16</v>
       </c>
-      <c r="M5" s="47">
+      <c r="M5" s="19">
         <v>651.36</v>
       </c>
-      <c r="N5" s="47">
+      <c r="N5" s="19">
         <v>887.80000000000007</v>
       </c>
-      <c r="O5" s="47">
+      <c r="O5" s="19">
         <v>1004.6400000000001</v>
       </c>
-      <c r="P5" s="47">
+      <c r="P5" s="19">
         <v>1146.32</v>
       </c>
-      <c r="Q5" s="47">
+      <c r="Q5" s="19">
         <v>1273.28</v>
       </c>
-      <c r="R5" s="47">
+      <c r="R5" s="19">
         <v>1373.5600000000002</v>
       </c>
-      <c r="S5" s="47">
+      <c r="S5" s="19">
         <v>287.04000000000002</v>
       </c>
-      <c r="T5" s="47">
+      <c r="T5" s="19">
         <v>319.24</v>
       </c>
-      <c r="U5" s="47">
+      <c r="U5" s="19">
         <v>343.16</v>
       </c>
     </row>
@@ -9742,64 +9739,64 @@
       <c r="A6" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="19">
         <v>225</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="19">
         <v>265</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="19">
         <v>267</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="19">
         <v>290</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="19">
         <v>301</v>
       </c>
-      <c r="G6" s="47">
+      <c r="G6" s="19">
         <v>316</v>
       </c>
-      <c r="H6" s="47">
+      <c r="H6" s="19">
         <v>339</v>
       </c>
-      <c r="I6" s="47">
+      <c r="I6" s="19">
         <v>369</v>
       </c>
-      <c r="J6" s="47">
+      <c r="J6" s="19">
         <v>397</v>
       </c>
-      <c r="K6" s="47">
+      <c r="K6" s="19">
         <v>456</v>
       </c>
-      <c r="L6" s="47">
+      <c r="L6" s="19">
         <v>456</v>
       </c>
-      <c r="M6" s="47">
+      <c r="M6" s="19">
         <v>588</v>
       </c>
-      <c r="N6" s="47">
+      <c r="N6" s="19">
         <v>737</v>
       </c>
-      <c r="O6" s="47">
+      <c r="O6" s="19">
         <v>851</v>
       </c>
-      <c r="P6" s="47">
+      <c r="P6" s="19">
         <v>968</v>
       </c>
-      <c r="Q6" s="47">
+      <c r="Q6" s="19">
         <v>1093</v>
       </c>
-      <c r="R6" s="47">
+      <c r="R6" s="19">
         <v>1211</v>
       </c>
-      <c r="S6" s="47">
+      <c r="S6" s="19">
         <v>260</v>
       </c>
-      <c r="T6" s="47">
+      <c r="T6" s="19">
         <v>318</v>
       </c>
-      <c r="U6" s="47">
+      <c r="U6" s="19">
         <v>341</v>
       </c>
     </row>
@@ -9807,64 +9804,64 @@
       <c r="A7" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="19">
         <v>176</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="19">
         <v>211</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="19">
         <v>213</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="19">
         <v>229</v>
       </c>
-      <c r="F7" s="47">
+      <c r="F7" s="19">
         <v>237</v>
       </c>
-      <c r="G7" s="47">
+      <c r="G7" s="19">
         <v>253</v>
       </c>
-      <c r="H7" s="47">
+      <c r="H7" s="19">
         <v>272</v>
       </c>
-      <c r="I7" s="47">
+      <c r="I7" s="19">
         <v>290</v>
       </c>
-      <c r="J7" s="47">
+      <c r="J7" s="19">
         <v>320</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="19">
         <v>343</v>
       </c>
-      <c r="L7" s="47">
+      <c r="L7" s="19">
         <v>365</v>
       </c>
-      <c r="M7" s="47">
+      <c r="M7" s="19">
         <v>448</v>
       </c>
-      <c r="N7" s="47">
+      <c r="N7" s="19">
         <v>562</v>
       </c>
-      <c r="O7" s="47">
+      <c r="O7" s="19">
         <v>650</v>
       </c>
-      <c r="P7" s="47">
+      <c r="P7" s="19">
         <v>744</v>
       </c>
-      <c r="Q7" s="47">
+      <c r="Q7" s="19">
         <v>832</v>
       </c>
-      <c r="R7" s="47">
+      <c r="R7" s="19">
         <v>929</v>
       </c>
-      <c r="S7" s="47">
+      <c r="S7" s="19">
         <v>205</v>
       </c>
-      <c r="T7" s="47">
+      <c r="T7" s="19">
         <v>232</v>
       </c>
-      <c r="U7" s="47">
+      <c r="U7" s="19">
         <v>254</v>
       </c>
     </row>
@@ -9872,64 +9869,64 @@
       <c r="A8" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="47">
-        <v>663.58089763779526</v>
-      </c>
-      <c r="C8" s="47">
+      <c r="B8" s="19">
+        <v>663.58089763779503</v>
+      </c>
+      <c r="C8" s="19">
         <v>731.48342519685036</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="19">
         <v>744</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="19">
         <v>800.10564960629927</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="19">
         <v>825.04724409448818</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="19">
         <v>894.80627165354326</v>
       </c>
-      <c r="H8" s="47">
+      <c r="H8" s="19">
         <v>953.31014173228345</v>
       </c>
-      <c r="I8" s="47">
+      <c r="I8" s="19">
         <v>1055.1424999999999</v>
       </c>
-      <c r="J8" s="47">
+      <c r="J8" s="19">
         <v>1112.7710236220473</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="19">
         <v>1250.1141732283465</v>
       </c>
-      <c r="L8" s="47">
+      <c r="L8" s="19">
         <v>1481.9745590551181</v>
       </c>
-      <c r="M8" s="47">
+      <c r="M8" s="19">
         <v>2021.2124173228347</v>
       </c>
-      <c r="N8" s="47">
+      <c r="N8" s="19">
         <v>2322.3548818897639</v>
       </c>
-      <c r="O8" s="47">
+      <c r="O8" s="19">
         <v>2900.5342913385825</v>
       </c>
-      <c r="P8" s="47">
+      <c r="P8" s="19">
         <v>3733.5348031496064</v>
       </c>
-      <c r="Q8" s="47">
+      <c r="Q8" s="19">
         <v>4624.628681102362</v>
       </c>
-      <c r="R8" s="47">
+      <c r="R8" s="19">
         <v>5052.4966141732284</v>
       </c>
-      <c r="S8" s="47">
+      <c r="S8" s="19">
         <v>828.42519685039372</v>
       </c>
-      <c r="T8" s="47">
+      <c r="T8" s="19">
         <v>909.54283464566925</v>
       </c>
-      <c r="U8" s="47">
+      <c r="U8" s="19">
         <v>983.93275590551184</v>
       </c>
     </row>
@@ -9937,64 +9934,64 @@
       <c r="A9" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B9" s="19">
         <v>534.58089763779526</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="19">
         <v>592.48342519685036</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="19">
         <v>601</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="19">
         <v>651.10564960629927</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F9" s="19">
         <v>664.04724409448818</v>
       </c>
-      <c r="G9" s="47">
+      <c r="G9" s="19">
         <v>721.80627165354326</v>
       </c>
-      <c r="H9" s="47">
+      <c r="H9" s="19">
         <v>774.31014173228345</v>
       </c>
-      <c r="I9" s="47">
+      <c r="I9" s="19">
         <v>862.14250000000004</v>
       </c>
-      <c r="J9" s="47">
+      <c r="J9" s="19">
         <v>903.77102362204721</v>
       </c>
-      <c r="K9" s="47">
+      <c r="K9" s="19">
         <v>1018.1141732283464</v>
       </c>
-      <c r="L9" s="47">
+      <c r="L9" s="19">
         <v>1219.9745590551181</v>
       </c>
-      <c r="M9" s="47">
+      <c r="M9" s="19">
         <v>1583.2124173228347</v>
       </c>
-      <c r="N9" s="47">
+      <c r="N9" s="19">
         <v>1819.3548818897639</v>
       </c>
-      <c r="O9" s="47">
+      <c r="O9" s="19">
         <v>2283.5342913385825</v>
       </c>
-      <c r="P9" s="47">
+      <c r="P9" s="19">
         <v>2927.5348031496064</v>
       </c>
-      <c r="Q9" s="47">
+      <c r="Q9" s="19">
         <v>3629.628681102362</v>
       </c>
-      <c r="R9" s="47">
+      <c r="R9" s="19">
         <v>3951.4966141732284</v>
       </c>
-      <c r="S9" s="47">
+      <c r="S9" s="19">
         <v>650.42519685039372</v>
       </c>
-      <c r="T9" s="47">
+      <c r="T9" s="19">
         <v>723.54283464566925</v>
       </c>
-      <c r="U9" s="47">
+      <c r="U9" s="19">
         <v>783.93275590551184</v>
       </c>
     </row>
@@ -10002,64 +9999,64 @@
       <c r="A10" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B10" s="19">
         <v>819.9656535433071</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="19">
         <v>898.71561023622041</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="19">
         <v>907</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="19">
         <v>975.66234251968501</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="19">
         <v>999.26614173228347</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="19">
         <v>1099.2697244094488</v>
       </c>
-      <c r="H10" s="47">
+      <c r="H10" s="19">
         <v>1163.8107874015748</v>
       </c>
-      <c r="I10" s="47">
+      <c r="I10" s="19">
         <v>1274.8409448818898</v>
       </c>
-      <c r="J10" s="47">
+      <c r="J10" s="19">
         <v>1353.8907086614172</v>
       </c>
-      <c r="K10" s="47">
+      <c r="K10" s="19">
         <v>1543.0157480314961</v>
       </c>
-      <c r="L10" s="47">
+      <c r="L10" s="19">
         <v>1888.5336023622046</v>
       </c>
-      <c r="M10" s="47">
+      <c r="M10" s="19">
         <v>2640.0615551181104</v>
       </c>
-      <c r="N10" s="47">
+      <c r="N10" s="19">
         <v>3052.1442519685038</v>
       </c>
-      <c r="O10" s="47">
+      <c r="O10" s="19">
         <v>3830.7988582677162</v>
       </c>
-      <c r="P10" s="47">
+      <c r="P10" s="19">
         <v>4913.0863779527563</v>
       </c>
-      <c r="Q10" s="47">
+      <c r="Q10" s="19">
         <v>6319.4771062992131</v>
       </c>
-      <c r="R10" s="47">
+      <c r="R10" s="19">
         <v>6893.883622047244</v>
       </c>
-      <c r="S10" s="47">
+      <c r="S10" s="19">
         <v>1017.511811023622</v>
       </c>
-      <c r="T10" s="47">
+      <c r="T10" s="19">
         <v>1128.0822047244094</v>
       </c>
-      <c r="U10" s="47">
+      <c r="U10" s="19">
         <v>1229.128346456693</v>
       </c>
     </row>
@@ -10067,64 +10064,64 @@
       <c r="A11" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="19">
         <v>659.9656535433071</v>
       </c>
-      <c r="C11" s="47">
+      <c r="C11" s="19">
         <v>727.71561023622041</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="19">
         <v>737</v>
       </c>
-      <c r="E11" s="47">
+      <c r="E11" s="19">
         <v>797.66234251968501</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F11" s="19">
         <v>807.26614173228347</v>
       </c>
-      <c r="G11" s="47">
+      <c r="G11" s="19">
         <v>890.26972440944883</v>
       </c>
-      <c r="H11" s="47">
+      <c r="H11" s="19">
         <v>943.81078740157477</v>
       </c>
-      <c r="I11" s="47">
+      <c r="I11" s="19">
         <v>1045.8409448818898</v>
       </c>
-      <c r="J11" s="47">
+      <c r="J11" s="19">
         <v>1100.8907086614172</v>
       </c>
-      <c r="K11" s="47">
+      <c r="K11" s="19">
         <v>1257.0157480314961</v>
       </c>
-      <c r="L11" s="47">
+      <c r="L11" s="19">
         <v>1537.5336023622046</v>
       </c>
-      <c r="M11" s="47">
+      <c r="M11" s="19">
         <v>2078.0615551181104</v>
       </c>
-      <c r="N11" s="47">
+      <c r="N11" s="19">
         <v>2406.1442519685038</v>
       </c>
-      <c r="O11" s="47">
+      <c r="O11" s="19">
         <v>3027.7988582677162</v>
       </c>
-      <c r="P11" s="47">
+      <c r="P11" s="19">
         <v>3853.0863779527563</v>
       </c>
-      <c r="Q11" s="47">
+      <c r="Q11" s="19">
         <v>4974.4771062992131</v>
       </c>
-      <c r="R11" s="47">
+      <c r="R11" s="19">
         <v>5414.883622047244</v>
       </c>
-      <c r="S11" s="47">
+      <c r="S11" s="19">
         <v>812.51181102362204</v>
       </c>
-      <c r="T11" s="47">
+      <c r="T11" s="19">
         <v>911.08220472440951</v>
       </c>
-      <c r="U11" s="47">
+      <c r="U11" s="19">
         <v>986.12834645669295</v>
       </c>
     </row>
@@ -10132,64 +10129,64 @@
       <c r="A12" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="47">
+      <c r="B12" s="19">
         <v>625</v>
       </c>
-      <c r="C12" s="47">
+      <c r="C12" s="19">
         <v>714</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="19">
         <v>742</v>
       </c>
-      <c r="E12" s="47">
+      <c r="E12" s="19">
         <v>803</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="19">
         <v>840</v>
       </c>
-      <c r="G12" s="47">
+      <c r="G12" s="19">
         <v>905</v>
       </c>
-      <c r="H12" s="47">
+      <c r="H12" s="19">
         <v>971</v>
       </c>
-      <c r="I12" s="47">
+      <c r="I12" s="19">
         <v>1043</v>
       </c>
-      <c r="J12" s="47">
+      <c r="J12" s="19">
         <v>1112</v>
       </c>
-      <c r="K12" s="47">
+      <c r="K12" s="19">
         <v>1225.8</v>
       </c>
-      <c r="L12" s="47">
+      <c r="L12" s="19">
         <v>1347.8</v>
       </c>
-      <c r="M12" s="47">
+      <c r="M12" s="19">
         <v>1762.2124173228347</v>
       </c>
-      <c r="N12" s="47">
+      <c r="N12" s="19">
         <v>2003.3548818897639</v>
       </c>
-      <c r="O12" s="47">
+      <c r="O12" s="19">
         <v>2396.5342913385825</v>
       </c>
-      <c r="P12" s="47">
+      <c r="P12" s="19">
         <v>2934.5348031496064</v>
       </c>
-      <c r="Q12" s="47">
+      <c r="Q12" s="19">
         <v>3645.628681102362</v>
       </c>
-      <c r="R12" s="47">
+      <c r="R12" s="19">
         <v>4150.4966141732284</v>
       </c>
-      <c r="S12" s="47">
+      <c r="S12" s="19">
         <v>704.4</v>
       </c>
-      <c r="T12" s="47">
+      <c r="T12" s="19">
         <v>804.8</v>
       </c>
-      <c r="U12" s="47">
+      <c r="U12" s="19">
         <v>838</v>
       </c>
     </row>
@@ -10197,64 +10194,64 @@
       <c r="A13" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B13" s="19">
         <v>510</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="19">
         <v>580</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="19">
         <v>601</v>
       </c>
-      <c r="E13" s="47">
+      <c r="E13" s="19">
         <v>654</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F13" s="19">
         <v>686</v>
       </c>
-      <c r="G13" s="47">
+      <c r="G13" s="19">
         <v>744</v>
       </c>
-      <c r="H13" s="47">
+      <c r="H13" s="19">
         <v>795</v>
       </c>
-      <c r="I13" s="47">
+      <c r="I13" s="19">
         <v>858</v>
       </c>
-      <c r="J13" s="47">
+      <c r="J13" s="19">
         <v>903</v>
       </c>
-      <c r="K13" s="47">
+      <c r="K13" s="19">
         <v>999.8</v>
       </c>
-      <c r="L13" s="47">
+      <c r="L13" s="19">
         <v>1099.8</v>
       </c>
-      <c r="M13" s="47">
+      <c r="M13" s="19">
         <v>1388.2124173228347</v>
       </c>
-      <c r="N13" s="47">
+      <c r="N13" s="19">
         <v>1578.3548818897639</v>
       </c>
-      <c r="O13" s="47">
+      <c r="O13" s="19">
         <v>1893.5342913385825</v>
       </c>
-      <c r="P13" s="47">
+      <c r="P13" s="19">
         <v>2309.5348031496064</v>
       </c>
-      <c r="Q13" s="47">
+      <c r="Q13" s="19">
         <v>2878.628681102362</v>
       </c>
-      <c r="R13" s="47">
+      <c r="R13" s="19">
         <v>3265.4966141732284</v>
       </c>
-      <c r="S13" s="47">
+      <c r="S13" s="19">
         <v>550.4</v>
       </c>
-      <c r="T13" s="47">
+      <c r="T13" s="19">
         <v>644.79999999999995</v>
       </c>
-      <c r="U13" s="47">
+      <c r="U13" s="19">
         <v>705</v>
       </c>
     </row>
@@ -10262,64 +10259,64 @@
       <c r="A14" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="19">
         <v>353.2</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="19">
         <v>373.6</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="19">
         <v>390</v>
       </c>
-      <c r="E14" s="47">
+      <c r="E14" s="19">
         <v>421.4</v>
       </c>
-      <c r="F14" s="47">
+      <c r="F14" s="19">
         <v>443.8</v>
       </c>
-      <c r="G14" s="47">
+      <c r="G14" s="19">
         <v>449.2</v>
       </c>
-      <c r="H14" s="47">
+      <c r="H14" s="19">
         <v>468</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="19">
         <v>476</v>
       </c>
-      <c r="J14" s="47">
+      <c r="J14" s="19">
         <v>485</v>
       </c>
-      <c r="K14" s="47">
+      <c r="K14" s="19">
         <v>519</v>
       </c>
-      <c r="L14" s="47">
+      <c r="L14" s="19">
         <v>566</v>
       </c>
-      <c r="M14" s="47">
+      <c r="M14" s="19">
         <v>729.2</v>
       </c>
-      <c r="N14" s="47">
+      <c r="N14" s="19">
         <v>803</v>
       </c>
-      <c r="O14" s="47">
+      <c r="O14" s="19">
         <v>884</v>
       </c>
-      <c r="P14" s="47">
+      <c r="P14" s="19">
         <v>1111</v>
       </c>
-      <c r="Q14" s="47">
+      <c r="Q14" s="19">
         <v>1491</v>
       </c>
-      <c r="R14" s="47">
+      <c r="R14" s="19">
         <v>1879</v>
       </c>
-      <c r="S14" s="47">
+      <c r="S14" s="19">
         <v>412</v>
       </c>
-      <c r="T14" s="47">
+      <c r="T14" s="19">
         <v>446</v>
       </c>
-      <c r="U14" s="47">
+      <c r="U14" s="19">
         <v>466</v>
       </c>
     </row>
@@ -10327,64 +10324,64 @@
       <c r="A15" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="47">
+      <c r="B15" s="19">
         <v>290.2</v>
       </c>
-      <c r="C15" s="47">
+      <c r="C15" s="19">
         <v>305.60000000000002</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="19">
         <v>315</v>
       </c>
-      <c r="E15" s="47">
+      <c r="E15" s="19">
         <v>343.4</v>
       </c>
-      <c r="F15" s="47">
+      <c r="F15" s="19">
         <v>363.8</v>
       </c>
-      <c r="G15" s="47">
+      <c r="G15" s="19">
         <v>366.2</v>
       </c>
-      <c r="H15" s="47">
+      <c r="H15" s="19">
         <v>380</v>
       </c>
-      <c r="I15" s="47">
+      <c r="I15" s="19">
         <v>385</v>
       </c>
-      <c r="J15" s="47">
+      <c r="J15" s="19">
         <v>391</v>
       </c>
-      <c r="K15" s="47">
+      <c r="K15" s="19">
         <v>421</v>
       </c>
-      <c r="L15" s="47">
+      <c r="L15" s="19">
         <v>463</v>
       </c>
-      <c r="M15" s="47">
+      <c r="M15" s="19">
         <v>574.20000000000005</v>
       </c>
-      <c r="N15" s="47">
+      <c r="N15" s="19">
         <v>637</v>
       </c>
-      <c r="O15" s="47">
+      <c r="O15" s="19">
         <v>704</v>
       </c>
-      <c r="P15" s="47">
+      <c r="P15" s="19">
         <v>883</v>
       </c>
-      <c r="Q15" s="47">
+      <c r="Q15" s="19">
         <v>1175</v>
       </c>
-      <c r="R15" s="47">
+      <c r="R15" s="19">
         <v>1484</v>
       </c>
-      <c r="S15" s="47">
+      <c r="S15" s="19">
         <v>327</v>
       </c>
-      <c r="T15" s="47">
+      <c r="T15" s="19">
         <v>352</v>
       </c>
-      <c r="U15" s="47">
+      <c r="U15" s="19">
         <v>386</v>
       </c>
     </row>
@@ -10392,64 +10389,64 @@
       <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="19">
         <v>628</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="19">
         <v>673</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D16" s="19">
         <v>677</v>
       </c>
-      <c r="E16" s="47">
+      <c r="E16" s="19">
         <v>728</v>
       </c>
-      <c r="F16" s="47">
+      <c r="F16" s="19">
         <v>760</v>
       </c>
-      <c r="G16" s="47">
+      <c r="G16" s="19">
         <v>813</v>
       </c>
-      <c r="H16" s="47">
+      <c r="H16" s="19">
         <v>882</v>
       </c>
-      <c r="I16" s="47">
+      <c r="I16" s="19">
         <v>937</v>
       </c>
-      <c r="J16" s="47">
+      <c r="J16" s="19">
         <v>1009</v>
       </c>
-      <c r="K16" s="47">
+      <c r="K16" s="19">
         <v>1137</v>
       </c>
-      <c r="L16" s="47">
+      <c r="L16" s="19">
         <v>1251</v>
       </c>
-      <c r="M16" s="47">
+      <c r="M16" s="19">
         <v>1650</v>
       </c>
-      <c r="N16" s="47">
+      <c r="N16" s="19">
         <v>1929</v>
       </c>
-      <c r="O16" s="47">
+      <c r="O16" s="19">
         <v>2385</v>
       </c>
-      <c r="P16" s="47">
+      <c r="P16" s="19">
         <v>3132</v>
       </c>
-      <c r="Q16" s="47">
+      <c r="Q16" s="19">
         <v>3821</v>
       </c>
-      <c r="R16" s="47">
+      <c r="R16" s="19">
         <v>4211</v>
       </c>
-      <c r="S16" s="47">
+      <c r="S16" s="19">
         <v>700</v>
       </c>
-      <c r="T16" s="47">
+      <c r="T16" s="19">
         <v>819</v>
       </c>
-      <c r="U16" s="47">
+      <c r="U16" s="19">
         <v>884</v>
       </c>
     </row>
@@ -10457,64 +10454,64 @@
       <c r="A17" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="47">
+      <c r="B17" s="19">
         <v>499</v>
       </c>
-      <c r="C17" s="47">
+      <c r="C17" s="19">
         <v>531</v>
       </c>
-      <c r="D17" s="47">
+      <c r="D17" s="19">
         <v>534</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="19">
         <v>579</v>
       </c>
-      <c r="F17" s="47">
+      <c r="F17" s="19">
         <v>603</v>
       </c>
-      <c r="G17" s="47">
+      <c r="G17" s="19">
         <v>640</v>
       </c>
-      <c r="H17" s="47">
+      <c r="H17" s="19">
         <v>703</v>
       </c>
-      <c r="I17" s="47">
+      <c r="I17" s="19">
         <v>742</v>
       </c>
-      <c r="J17" s="47">
+      <c r="J17" s="19">
         <v>798</v>
       </c>
-      <c r="K17" s="47">
+      <c r="K17" s="19">
         <v>901</v>
       </c>
-      <c r="L17" s="47">
+      <c r="L17" s="19">
         <v>985</v>
       </c>
-      <c r="M17" s="47">
+      <c r="M17" s="19">
         <v>1263</v>
       </c>
-      <c r="N17" s="47">
+      <c r="N17" s="19">
         <v>1476</v>
       </c>
-      <c r="O17" s="47">
+      <c r="O17" s="19">
         <v>1828</v>
       </c>
-      <c r="P17" s="47">
+      <c r="P17" s="19">
         <v>2402</v>
       </c>
-      <c r="Q17" s="47">
+      <c r="Q17" s="19">
         <v>2928</v>
       </c>
-      <c r="R17" s="47">
+      <c r="R17" s="19">
         <v>3230</v>
       </c>
-      <c r="S17" s="47">
+      <c r="S17" s="19">
         <v>551</v>
       </c>
-      <c r="T17" s="47">
+      <c r="T17" s="19">
         <v>641</v>
       </c>
-      <c r="U17" s="47">
+      <c r="U17" s="19">
         <v>722</v>
       </c>
     </row>
@@ -10522,64 +10519,64 @@
       <c r="A18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="47">
+      <c r="B18" s="19">
         <v>232</v>
       </c>
-      <c r="C18" s="47">
+      <c r="C18" s="19">
         <v>252</v>
       </c>
-      <c r="D18" s="47">
+      <c r="D18" s="19">
         <v>263</v>
       </c>
-      <c r="E18" s="47">
+      <c r="E18" s="19">
         <v>290</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F18" s="19">
         <v>316</v>
       </c>
-      <c r="G18" s="47">
+      <c r="G18" s="19">
         <v>316</v>
       </c>
-      <c r="H18" s="47">
+      <c r="H18" s="19">
         <v>341</v>
       </c>
-      <c r="I18" s="47">
+      <c r="I18" s="19">
         <v>384</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="19">
         <v>391</v>
       </c>
-      <c r="K18" s="47">
+      <c r="K18" s="19">
         <v>404</v>
       </c>
-      <c r="L18" s="47">
+      <c r="L18" s="19">
         <v>450</v>
       </c>
-      <c r="M18" s="47">
+      <c r="M18" s="19">
         <v>593</v>
       </c>
-      <c r="N18" s="47">
+      <c r="N18" s="19">
         <v>674</v>
       </c>
-      <c r="O18" s="47">
+      <c r="O18" s="19">
         <v>737</v>
       </c>
-      <c r="P18" s="47">
+      <c r="P18" s="19">
         <v>790</v>
       </c>
-      <c r="Q18" s="47">
+      <c r="Q18" s="19">
         <v>902</v>
       </c>
-      <c r="R18" s="47">
+      <c r="R18" s="19">
         <v>950</v>
       </c>
-      <c r="S18" s="47">
+      <c r="S18" s="19">
         <v>292</v>
       </c>
-      <c r="T18" s="47">
+      <c r="T18" s="19">
         <v>318</v>
       </c>
-      <c r="U18" s="47">
+      <c r="U18" s="19">
         <v>352</v>
       </c>
     </row>
@@ -10587,64 +10584,64 @@
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19" s="19">
         <v>274</v>
       </c>
-      <c r="C19" s="47">
+      <c r="C19" s="19">
         <v>274</v>
       </c>
-      <c r="D19" s="47">
+      <c r="D19" s="19">
         <v>301</v>
       </c>
-      <c r="E19" s="47">
+      <c r="E19" s="19">
         <v>301</v>
       </c>
-      <c r="F19" s="47">
+      <c r="F19" s="19">
         <v>325</v>
       </c>
-      <c r="G19" s="47">
+      <c r="G19" s="19">
         <v>361</v>
       </c>
-      <c r="H19" s="47">
+      <c r="H19" s="19">
         <v>392</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="19">
         <v>450</v>
       </c>
-      <c r="J19" s="47">
+      <c r="J19" s="19">
         <v>509</v>
       </c>
-      <c r="K19" s="47">
+      <c r="K19" s="19">
         <v>573</v>
       </c>
-      <c r="L19" s="47">
+      <c r="L19" s="19">
         <v>687</v>
       </c>
-      <c r="M19" s="47">
+      <c r="M19" s="19">
         <v>963</v>
       </c>
-      <c r="N19" s="47">
+      <c r="N19" s="19">
         <v>1196</v>
       </c>
-      <c r="O19" s="47">
+      <c r="O19" s="19">
         <v>1383</v>
       </c>
-      <c r="P19" s="47">
+      <c r="P19" s="19">
         <v>1567</v>
       </c>
-      <c r="Q19" s="47">
+      <c r="Q19" s="19">
         <v>1775</v>
       </c>
-      <c r="R19" s="47">
+      <c r="R19" s="19">
         <v>1957</v>
       </c>
-      <c r="S19" s="47">
+      <c r="S19" s="19">
         <v>303</v>
       </c>
-      <c r="T19" s="47">
+      <c r="T19" s="19">
         <v>364</v>
       </c>
-      <c r="U19" s="47">
+      <c r="U19" s="19">
         <v>407</v>
       </c>
     </row>
@@ -10652,64 +10649,64 @@
       <c r="A20" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="47">
+      <c r="B20" s="19">
         <v>255</v>
       </c>
-      <c r="C20" s="47">
+      <c r="C20" s="19">
         <v>255</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D20" s="19">
         <v>283</v>
       </c>
-      <c r="E20" s="47">
+      <c r="E20" s="19">
         <v>283</v>
       </c>
-      <c r="F20" s="47">
+      <c r="F20" s="19">
         <v>309</v>
       </c>
-      <c r="G20" s="47">
+      <c r="G20" s="19">
         <v>338</v>
       </c>
-      <c r="H20" s="47">
+      <c r="H20" s="19">
         <v>368</v>
       </c>
-      <c r="I20" s="47">
+      <c r="I20" s="19">
         <v>423</v>
       </c>
-      <c r="J20" s="47">
+      <c r="J20" s="19">
         <v>478</v>
       </c>
-      <c r="K20" s="47">
+      <c r="K20" s="19">
         <v>526</v>
       </c>
-      <c r="L20" s="47">
+      <c r="L20" s="19">
         <v>642</v>
       </c>
-      <c r="M20" s="47">
+      <c r="M20" s="19">
         <v>869</v>
       </c>
-      <c r="N20" s="47">
+      <c r="N20" s="19">
         <v>1079</v>
       </c>
-      <c r="O20" s="47">
+      <c r="O20" s="19">
         <v>1255</v>
       </c>
-      <c r="P20" s="47">
+      <c r="P20" s="19">
         <v>1411</v>
       </c>
-      <c r="Q20" s="47">
+      <c r="Q20" s="19">
         <v>1602</v>
       </c>
-      <c r="R20" s="47">
+      <c r="R20" s="19">
         <v>1770</v>
       </c>
-      <c r="S20" s="47">
+      <c r="S20" s="19">
         <v>283</v>
       </c>
-      <c r="T20" s="47">
+      <c r="T20" s="19">
         <v>338</v>
       </c>
-      <c r="U20" s="47">
+      <c r="U20" s="19">
         <v>381</v>
       </c>
     </row>
@@ -10717,64 +10714,64 @@
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="47">
+      <c r="B21" s="19">
         <v>209</v>
       </c>
-      <c r="C21" s="47">
+      <c r="C21" s="19">
         <v>225</v>
       </c>
-      <c r="D21" s="47">
+      <c r="D21" s="19">
         <v>243</v>
       </c>
-      <c r="E21" s="47">
+      <c r="E21" s="19">
         <v>258</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F21" s="19">
         <v>287</v>
       </c>
-      <c r="G21" s="47">
+      <c r="G21" s="19">
         <v>296</v>
       </c>
-      <c r="H21" s="47">
+      <c r="H21" s="19">
         <v>312</v>
       </c>
-      <c r="I21" s="47">
+      <c r="I21" s="19">
         <v>342</v>
       </c>
-      <c r="J21" s="47">
+      <c r="J21" s="19">
         <v>371</v>
       </c>
-      <c r="K21" s="47">
+      <c r="K21" s="19">
         <v>393</v>
       </c>
-      <c r="L21" s="47">
+      <c r="L21" s="19">
         <v>421</v>
       </c>
-      <c r="M21" s="47">
+      <c r="M21" s="19">
         <v>535</v>
       </c>
-      <c r="N21" s="47" t="s">
+      <c r="N21" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="O21" s="47" t="s">
+      <c r="O21" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="P21" s="47" t="s">
+      <c r="P21" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="Q21" s="47" t="s">
+      <c r="Q21" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="R21" s="47" t="s">
+      <c r="R21" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="S21" s="47">
+      <c r="S21" s="19">
         <v>256</v>
       </c>
-      <c r="T21" s="47">
+      <c r="T21" s="19">
         <v>265</v>
       </c>
-      <c r="U21" s="47">
+      <c r="U21" s="19">
         <v>285</v>
       </c>
     </row>
@@ -10782,64 +10779,64 @@
       <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="47">
+      <c r="B22" s="19">
         <v>763</v>
       </c>
-      <c r="C22" s="47">
+      <c r="C22" s="19">
         <v>763</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="19">
         <v>825</v>
       </c>
-      <c r="E22" s="47">
+      <c r="E22" s="19">
         <v>883</v>
       </c>
-      <c r="F22" s="47">
+      <c r="F22" s="19">
         <v>923</v>
       </c>
-      <c r="G22" s="47">
+      <c r="G22" s="19">
         <v>987</v>
       </c>
-      <c r="H22" s="47">
+      <c r="H22" s="19">
         <v>1034</v>
       </c>
-      <c r="I22" s="47">
+      <c r="I22" s="19">
         <v>1119</v>
       </c>
-      <c r="J22" s="47">
+      <c r="J22" s="19">
         <v>1307</v>
       </c>
-      <c r="K22" s="47">
+      <c r="K22" s="19">
         <v>1379</v>
       </c>
-      <c r="L22" s="47">
+      <c r="L22" s="19">
         <v>1571</v>
       </c>
-      <c r="M22" s="47">
+      <c r="M22" s="19">
         <v>2135</v>
       </c>
-      <c r="N22" s="47">
+      <c r="N22" s="19">
         <v>2559</v>
       </c>
-      <c r="O22" s="47">
+      <c r="O22" s="19">
         <v>2994</v>
       </c>
-      <c r="P22" s="47" t="s">
+      <c r="P22" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="Q22" s="47" t="s">
+      <c r="Q22" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="R22" s="47" t="s">
+      <c r="R22" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="S22" s="47">
+      <c r="S22" s="19">
         <v>836</v>
       </c>
-      <c r="T22" s="47">
+      <c r="T22" s="19">
         <v>995</v>
       </c>
-      <c r="U22" s="47">
+      <c r="U22" s="19">
         <v>1062</v>
       </c>
     </row>
@@ -10847,64 +10844,64 @@
       <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="47">
+      <c r="B23" s="19">
         <v>432</v>
       </c>
-      <c r="C23" s="47">
+      <c r="C23" s="19">
         <v>470</v>
       </c>
-      <c r="D23" s="47">
+      <c r="D23" s="19">
         <v>470</v>
       </c>
-      <c r="E23" s="47">
+      <c r="E23" s="19">
         <v>515</v>
       </c>
-      <c r="F23" s="47">
+      <c r="F23" s="19">
         <v>515</v>
       </c>
-      <c r="G23" s="47">
+      <c r="G23" s="19">
         <v>555</v>
       </c>
-      <c r="H23" s="47">
+      <c r="H23" s="19">
         <v>559</v>
       </c>
-      <c r="I23" s="47">
+      <c r="I23" s="19">
         <v>614</v>
       </c>
-      <c r="J23" s="47">
+      <c r="J23" s="19">
         <v>632</v>
       </c>
-      <c r="K23" s="47">
+      <c r="K23" s="19">
         <v>676</v>
       </c>
-      <c r="L23" s="47">
+      <c r="L23" s="19">
         <v>715</v>
       </c>
-      <c r="M23" s="47">
+      <c r="M23" s="19">
         <v>983</v>
       </c>
-      <c r="N23" s="47">
+      <c r="N23" s="19">
         <v>1102</v>
       </c>
-      <c r="O23" s="47">
+      <c r="O23" s="19">
         <v>1257</v>
       </c>
-      <c r="P23" s="47">
+      <c r="P23" s="19">
         <v>1365</v>
       </c>
-      <c r="Q23" s="47">
+      <c r="Q23" s="19">
         <v>1527</v>
       </c>
-      <c r="R23" s="47">
+      <c r="R23" s="19">
         <v>1637</v>
       </c>
-      <c r="S23" s="47">
+      <c r="S23" s="19">
         <v>518</v>
       </c>
-      <c r="T23" s="47">
+      <c r="T23" s="19">
         <v>574</v>
       </c>
-      <c r="U23" s="47">
+      <c r="U23" s="19">
         <v>619</v>
       </c>
     </row>
@@ -10933,100 +10930,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="53"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="52"/>
     </row>
     <row r="2" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="50"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="49"/>
       <c r="T2" s="25"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="58"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="57"/>
     </row>
     <row r="4" spans="1:20" s="16" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63"/>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="64"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="63"/>
     </row>
     <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="60"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
       <c r="D5" s="33"/>
@@ -11047,7 +11044,7 @@
       <c r="S5" s="34"/>
     </row>
     <row r="6" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="61"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="35">
         <v>100</v>
       </c>
@@ -12166,8 +12163,8 @@
       </c>
     </row>
     <row r="25" spans="1:19" ht="18" x14ac:dyDescent="0.15">
-      <c r="A25" s="65"/>
-      <c r="B25" s="66"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="65"/>
       <c r="C25" s="43"/>
       <c r="D25" s="44"/>
       <c r="E25" s="43"/>
@@ -12187,23 +12184,23 @@
       <c r="S25" s="10"/>
     </row>
     <row r="26" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="54"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="55"/>
+      <c r="A26" s="53"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="54"/>
+      <c r="Q26" s="54"/>
       <c r="R26" s="9"/>
       <c r="S26" s="10"/>
     </row>
@@ -12229,25 +12226,25 @@
       <c r="S27" s="10"/>
     </row>
     <row r="28" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="55"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="54"/>
+      <c r="M28" s="54"/>
+      <c r="N28" s="54"/>
+      <c r="O28" s="54"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
       <c r="R28" s="9"/>
       <c r="S28" s="10"/>
     </row>
@@ -12309,90 +12306,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="75"/>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
       <c r="S1" s="10"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="72"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="71"/>
     </row>
     <row r="3" spans="1:20" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="48"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="50"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="49"/>
       <c r="T3" s="25"/>
     </row>
     <row r="4" spans="1:20" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="9"/>
       <c r="S4" s="23"/>
@@ -13150,48 +13147,48 @@
       <c r="S18" s="10"/>
     </row>
     <row r="19" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="67"/>
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
-      <c r="M19" s="68"/>
-      <c r="N19" s="68"/>
-      <c r="O19" s="68"/>
-      <c r="P19" s="68"/>
-      <c r="Q19" s="68"/>
-      <c r="R19" s="68"/>
-      <c r="S19" s="69"/>
+      <c r="A19" s="66"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="67"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="67"/>
+      <c r="S19" s="68"/>
     </row>
     <row r="20" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="57"/>
-      <c r="P20" s="57"/>
-      <c r="Q20" s="57"/>
-      <c r="R20" s="57"/>
-      <c r="S20" s="58"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="56"/>
+      <c r="P20" s="56"/>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="56"/>
+      <c r="S20" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -13229,72 +13226,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
       <c r="R1" s="5"/>
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="50"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="49"/>
       <c r="T2" s="25"/>
     </row>
     <row r="3" spans="1:20" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="83"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
       <c r="R3" s="11"/>
       <c r="S3" s="12"/>
     </row>
@@ -14774,48 +14771,48 @@
       </c>
     </row>
     <row r="29" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="54"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="55"/>
-      <c r="N29" s="55"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="55"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
+      <c r="O29" s="54"/>
+      <c r="P29" s="54"/>
+      <c r="Q29" s="54"/>
       <c r="R29" s="9"/>
       <c r="S29" s="10"/>
     </row>
     <row r="30" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="78"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="78"/>
-      <c r="J30" s="78"/>
-      <c r="K30" s="78"/>
-      <c r="L30" s="78"/>
-      <c r="M30" s="78"/>
-      <c r="N30" s="78"/>
-      <c r="O30" s="78"/>
-      <c r="P30" s="78"/>
-      <c r="Q30" s="78"/>
-      <c r="R30" s="78"/>
-      <c r="S30" s="79"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="77"/>
+      <c r="N30" s="77"/>
+      <c r="O30" s="77"/>
+      <c r="P30" s="77"/>
+      <c r="Q30" s="77"/>
+      <c r="R30" s="77"/>
+      <c r="S30" s="78"/>
     </row>
     <row r="31" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="31"/>

</xml_diff>